<commit_message>
dados do usuario no drawer e editar perfil + tabela de riscos atualizada
tive que remover o middleware na rota de edição do usuário para fazer a edição do mesmo.
</commit_message>
<xml_diff>
--- a/documentacao/TabelaRiscos.xlsx
+++ b/documentacao/TabelaRiscos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vinicius Piantoni\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TCC\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37D2FA1-8F64-4EF2-9C9A-800464255ED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -143,7 +144,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -318,9 +319,6 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -330,34 +328,13 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -366,6 +343,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -652,11 +653,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,489 +672,491 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="I3" s="14" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="I3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="14" t="s">
+      <c r="J3" s="10"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="14"/>
+      <c r="M3" s="10"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="12" t="s">
+      <c r="E4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="14" t="s">
+      <c r="G4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="14"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="16" t="s">
+      <c r="J4" s="10"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="M4" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3">
-        <v>5</v>
-      </c>
-      <c r="F5" s="3">
-        <v>3</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="E5" s="2">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2">
         <v>15</v>
       </c>
-      <c r="I5" s="15">
-        <v>5</v>
-      </c>
-      <c r="J5" s="17" t="s">
+      <c r="I5" s="7">
+        <v>5</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="16">
+      <c r="K5" s="6"/>
+      <c r="L5" s="8">
         <v>1</v>
       </c>
-      <c r="M5" s="16">
+      <c r="M5" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="3">
+      <c r="B6" s="14"/>
+      <c r="C6" s="2">
         <v>2</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="3">
-        <v>3</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2">
         <v>2</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>6</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="7">
         <v>4</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="16">
+      <c r="K6" s="6"/>
+      <c r="L6" s="8">
+        <v>3</v>
+      </c>
+      <c r="M6" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="15"/>
+      <c r="C7" s="3">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3">
+        <v>5</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3</v>
+      </c>
+      <c r="G7" s="3">
+        <v>15</v>
+      </c>
+      <c r="I7" s="7">
+        <v>3</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="6"/>
+      <c r="L7" s="8">
+        <v>9</v>
+      </c>
+      <c r="M7" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1">
         <v>2</v>
       </c>
-      <c r="M6" s="16">
+      <c r="F8" s="1">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="9"/>
-      <c r="C7" s="4">
-        <v>3</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="I8" s="7">
+        <v>2</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="6"/>
+      <c r="L8" s="8">
+        <v>10</v>
+      </c>
+      <c r="M8" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="14"/>
+      <c r="C9" s="2">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2</v>
+      </c>
+      <c r="G9" s="2">
+        <v>10</v>
+      </c>
+      <c r="I9" s="7">
+        <v>1</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="6"/>
+      <c r="L9" s="8">
+        <v>13</v>
+      </c>
+      <c r="M9" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="14"/>
+      <c r="C10" s="2">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>4</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="8">
+        <v>11</v>
+      </c>
+      <c r="M10" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="15"/>
+      <c r="C11" s="3">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>3</v>
+      </c>
+      <c r="G11" s="3">
+        <v>3</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="8">
+        <v>5</v>
+      </c>
+      <c r="M11" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>5</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="8">
+        <v>14</v>
+      </c>
+      <c r="M12" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="15"/>
+      <c r="C13" s="3">
         <v>9</v>
       </c>
-      <c r="E7" s="4">
-        <v>5</v>
-      </c>
-      <c r="F7" s="4">
-        <v>3</v>
-      </c>
-      <c r="G7" s="4">
+      <c r="D13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="3">
+        <v>5</v>
+      </c>
+      <c r="F13" s="3">
+        <v>3</v>
+      </c>
+      <c r="G13" s="3">
         <v>15</v>
       </c>
-      <c r="I7" s="15">
-        <v>3</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="16">
-        <v>3</v>
-      </c>
-      <c r="M7" s="16">
+      <c r="I13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="10"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="8">
+        <v>2</v>
+      </c>
+      <c r="M13" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1">
+        <v>5</v>
+      </c>
+      <c r="G14" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
+      <c r="I14" s="7">
+        <v>5</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14" s="6"/>
+      <c r="L14" s="8">
+        <v>4</v>
+      </c>
+      <c r="M14" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="14"/>
+      <c r="C15" s="2">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="2">
+        <v>4</v>
+      </c>
+      <c r="F15" s="2">
+        <v>3</v>
+      </c>
+      <c r="G15" s="2">
+        <v>12</v>
+      </c>
+      <c r="I15" s="7">
+        <v>4</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" s="6"/>
+      <c r="L15" s="8">
+        <v>8</v>
+      </c>
+      <c r="M15" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="15"/>
+      <c r="C16" s="3">
+        <v>12</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3">
+        <v>5</v>
+      </c>
+      <c r="G16" s="3">
+        <v>5</v>
+      </c>
+      <c r="I16" s="7">
+        <v>3</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K16" s="6"/>
+      <c r="L16" s="8">
+        <v>12</v>
+      </c>
+      <c r="M16" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="1">
+        <v>5</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1">
+        <v>15</v>
+      </c>
+      <c r="I17" s="7">
+        <v>2</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" s="6"/>
+      <c r="L17" s="8">
+        <v>6</v>
+      </c>
+      <c r="M17" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="17"/>
+      <c r="C18" s="2">
+        <v>14</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="2">
+        <v>5</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2</v>
+      </c>
+      <c r="G18" s="2">
         <v>10</v>
       </c>
-      <c r="C8" s="2">
-        <v>4</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="2">
-        <v>2</v>
-      </c>
-      <c r="F8" s="2">
-        <v>3</v>
-      </c>
-      <c r="G8" s="2">
-        <v>6</v>
-      </c>
-      <c r="I8" s="15">
-        <v>2</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" s="13"/>
-      <c r="L8" s="16">
-        <v>4</v>
-      </c>
-      <c r="M8" s="16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="3">
-        <v>5</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="3">
-        <v>5</v>
-      </c>
-      <c r="F9" s="3">
-        <v>2</v>
-      </c>
-      <c r="G9" s="3">
-        <v>10</v>
-      </c>
-      <c r="I9" s="15">
+      <c r="I18" s="7">
         <v>1</v>
       </c>
-      <c r="J9" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="K9" s="13"/>
-      <c r="L9" s="16">
-        <v>5</v>
-      </c>
-      <c r="M9" s="16">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="3">
-        <v>6</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="3">
-        <v>4</v>
-      </c>
-      <c r="F10" s="3">
-        <v>1</v>
-      </c>
-      <c r="G10" s="3">
-        <v>4</v>
-      </c>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="16">
-        <v>6</v>
-      </c>
-      <c r="M10" s="16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="9"/>
-      <c r="C11" s="4">
+      <c r="J18" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18" s="6"/>
+      <c r="L18" s="8">
         <v>7</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="4">
-        <v>1</v>
-      </c>
-      <c r="F11" s="4">
-        <v>3</v>
-      </c>
-      <c r="G11" s="4">
-        <v>3</v>
-      </c>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="16">
-        <v>7</v>
-      </c>
-      <c r="M11" s="16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="2">
-        <v>8</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="2">
-        <v>5</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1</v>
-      </c>
-      <c r="G12" s="2">
-        <v>5</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="J12" s="14"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="16">
-        <v>8</v>
-      </c>
-      <c r="M12" s="16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="9"/>
-      <c r="C13" s="4">
-        <v>9</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="4">
-        <v>5</v>
-      </c>
-      <c r="F13" s="4">
-        <v>3</v>
-      </c>
-      <c r="G13" s="4">
-        <v>15</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="14"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="16">
-        <v>9</v>
-      </c>
-      <c r="M13" s="16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="2">
-        <v>10</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="2">
-        <v>3</v>
-      </c>
-      <c r="F14" s="2">
-        <v>5</v>
-      </c>
-      <c r="G14" s="2">
-        <v>15</v>
-      </c>
-      <c r="I14" s="15">
-        <v>5</v>
-      </c>
-      <c r="J14" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="K14" s="13"/>
-      <c r="L14" s="16">
-        <v>10</v>
-      </c>
-      <c r="M14" s="16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="3">
-        <v>11</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="3">
-        <v>4</v>
-      </c>
-      <c r="F15" s="3">
-        <v>3</v>
-      </c>
-      <c r="G15" s="3">
-        <v>12</v>
-      </c>
-      <c r="I15" s="15">
-        <v>4</v>
-      </c>
-      <c r="J15" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="K15" s="13"/>
-      <c r="L15" s="16">
-        <v>11</v>
-      </c>
-      <c r="M15" s="16">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="9"/>
-      <c r="C16" s="4">
-        <v>12</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="4">
-        <v>1</v>
-      </c>
-      <c r="F16" s="4">
-        <v>5</v>
-      </c>
-      <c r="G16" s="4">
-        <v>5</v>
-      </c>
-      <c r="I16" s="15">
-        <v>3</v>
-      </c>
-      <c r="J16" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="K16" s="13"/>
-      <c r="L16" s="16">
-        <v>12</v>
-      </c>
-      <c r="M16" s="16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="2">
-        <v>13</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="2">
-        <v>5</v>
-      </c>
-      <c r="F17" s="2">
-        <v>3</v>
-      </c>
-      <c r="G17" s="2">
-        <v>15</v>
-      </c>
-      <c r="I17" s="15">
-        <v>2</v>
-      </c>
-      <c r="J17" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="K17" s="13"/>
-      <c r="L17" s="16">
-        <v>13</v>
-      </c>
-      <c r="M17" s="16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="11"/>
-      <c r="C18" s="3">
-        <v>14</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="3">
-        <v>5</v>
-      </c>
-      <c r="F18" s="3">
-        <v>2</v>
-      </c>
-      <c r="G18" s="3">
-        <v>10</v>
-      </c>
-      <c r="I18" s="15">
-        <v>1</v>
-      </c>
-      <c r="J18" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="K18" s="13"/>
-      <c r="L18" s="16">
-        <v>14</v>
-      </c>
-      <c r="M18" s="16">
-        <v>10</v>
+      <c r="M18" s="8">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B18"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="I4:J4"/>
@@ -1163,8 +1166,6 @@
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>